<commit_message>
Adequação Conforme NT 2024.001
</commit_message>
<xml_diff>
--- a/Emissão/Layouts/LAYOUT 3.0 CTe.xlsx
+++ b/Emissão/Layouts/LAYOUT 3.0 CTe.xlsx
@@ -2327,7 +2327,7 @@
     <t xml:space="preserve">Valor de ICMS de Desoneração</t>
   </si>
   <si>
-    <t xml:space="preserve">Deve ser informado quando for CST = 20, 45, 60, 90 ou OutraUF.</t>
+    <t xml:space="preserve">Deve ser informado quando for CST = 20, 40, 41, 51, 60 ou 90.</t>
   </si>
   <si>
     <t xml:space="preserve">4.0.0.0</t>
@@ -4983,7 +4983,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5006,6 +5006,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFFCD5B5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -5099,7 +5105,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="86">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5352,6 +5358,26 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5503,8 +5529,8 @@
   </sheetPr>
   <dimension ref="A1:AE1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G288" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J298" activeCellId="0" sqref="J298"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D276" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J297" activeCellId="0" sqref="J297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20694,38 +20720,38 @@
       <c r="AE296" s="4"/>
     </row>
     <row r="297" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A297" s="14" t="n">
+      <c r="A297" s="63" t="n">
         <f aca="false">A296+1</f>
         <v>217</v>
       </c>
-      <c r="B297" s="15" t="s">
+      <c r="B297" s="64" t="s">
         <v>740</v>
       </c>
-      <c r="C297" s="16" t="s">
+      <c r="C297" s="65" t="s">
         <v>741</v>
       </c>
-      <c r="D297" s="16" t="s">
+      <c r="D297" s="65" t="s">
         <v>742</v>
       </c>
-      <c r="E297" s="14" t="s">
+      <c r="E297" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="F297" s="14" t="s">
+      <c r="F297" s="63" t="s">
         <v>691</v>
       </c>
-      <c r="G297" s="14" t="s">
+      <c r="G297" s="63" t="s">
         <v>625</v>
       </c>
-      <c r="H297" s="17" t="s">
+      <c r="H297" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="I297" s="14" t="s">
+      <c r="I297" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="J297" s="62" t="s">
+      <c r="J297" s="67" t="s">
         <v>743</v>
       </c>
-      <c r="K297" s="15" t="s">
+      <c r="K297" s="64" t="s">
         <v>744</v>
       </c>
       <c r="L297" s="4"/>
@@ -20750,38 +20776,38 @@
       <c r="AE297" s="4"/>
     </row>
     <row r="298" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A298" s="14" t="n">
+      <c r="A298" s="63" t="n">
         <f aca="false">A297+1</f>
         <v>218</v>
       </c>
-      <c r="B298" s="15" t="s">
+      <c r="B298" s="64" t="s">
         <v>745</v>
       </c>
-      <c r="C298" s="16" t="s">
+      <c r="C298" s="65" t="s">
         <v>746</v>
       </c>
-      <c r="D298" s="16" t="s">
+      <c r="D298" s="65" t="s">
         <v>747</v>
       </c>
-      <c r="E298" s="14" t="s">
+      <c r="E298" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="F298" s="14" t="s">
+      <c r="F298" s="63" t="s">
         <v>691</v>
       </c>
-      <c r="G298" s="14" t="s">
+      <c r="G298" s="63" t="s">
         <v>748</v>
       </c>
-      <c r="H298" s="17" t="s">
+      <c r="H298" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="I298" s="14" t="s">
+      <c r="I298" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="J298" s="62" t="s">
+      <c r="J298" s="67" t="s">
         <v>743</v>
       </c>
-      <c r="K298" s="15" t="s">
+      <c r="K298" s="64" t="s">
         <v>744</v>
       </c>
       <c r="L298" s="4"/>
@@ -21867,7 +21893,7 @@
       <c r="I320" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J320" s="63" t="s">
+      <c r="J320" s="68" t="s">
         <v>327</v>
       </c>
       <c r="K320" s="15" t="s">
@@ -22143,7 +22169,7 @@
       <c r="I325" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J325" s="64"/>
+      <c r="J325" s="69"/>
       <c r="K325" s="15" t="s">
         <v>21</v>
       </c>
@@ -22197,7 +22223,7 @@
       <c r="I326" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J326" s="64"/>
+      <c r="J326" s="69"/>
       <c r="K326" s="15" t="s">
         <v>21</v>
       </c>
@@ -22251,7 +22277,7 @@
       <c r="I327" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J327" s="64" t="s">
+      <c r="J327" s="69" t="s">
         <v>343</v>
       </c>
       <c r="K327" s="15" t="s">
@@ -22307,7 +22333,7 @@
       <c r="I328" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J328" s="64" t="s">
+      <c r="J328" s="69" t="s">
         <v>630</v>
       </c>
       <c r="K328" s="15" t="s">
@@ -22363,7 +22389,7 @@
       <c r="I329" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J329" s="64" t="s">
+      <c r="J329" s="69" t="s">
         <v>630</v>
       </c>
       <c r="K329" s="15" t="s">
@@ -22419,7 +22445,7 @@
       <c r="I330" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J330" s="64" t="s">
+      <c r="J330" s="69" t="s">
         <v>630</v>
       </c>
       <c r="K330" s="15" t="s">
@@ -22475,7 +22501,7 @@
       <c r="I331" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J331" s="64" t="s">
+      <c r="J331" s="69" t="s">
         <v>630</v>
       </c>
       <c r="K331" s="15" t="s">
@@ -22531,7 +22557,7 @@
       <c r="I332" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J332" s="64" t="s">
+      <c r="J332" s="69" t="s">
         <v>630</v>
       </c>
       <c r="K332" s="15" t="s">
@@ -22587,7 +22613,7 @@
       <c r="I333" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J333" s="64" t="s">
+      <c r="J333" s="69" t="s">
         <v>630</v>
       </c>
       <c r="K333" s="15" t="s">
@@ -22699,7 +22725,7 @@
       <c r="I335" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J335" s="64" t="s">
+      <c r="J335" s="69" t="s">
         <v>630</v>
       </c>
       <c r="K335" s="15" t="s">
@@ -22755,7 +22781,7 @@
       <c r="I336" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J336" s="64" t="s">
+      <c r="J336" s="69" t="s">
         <v>849</v>
       </c>
       <c r="K336" s="15" t="s">
@@ -22811,7 +22837,7 @@
       <c r="I337" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J337" s="64" t="s">
+      <c r="J337" s="69" t="s">
         <v>343</v>
       </c>
       <c r="K337" s="15" t="s">
@@ -22867,7 +22893,7 @@
       <c r="I338" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J338" s="64"/>
+      <c r="J338" s="69"/>
       <c r="K338" s="15" t="s">
         <v>21</v>
       </c>
@@ -22921,7 +22947,7 @@
       <c r="I339" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J339" s="64" t="s">
+      <c r="J339" s="69" t="s">
         <v>849</v>
       </c>
       <c r="K339" s="15" t="s">
@@ -22977,7 +23003,7 @@
       <c r="I340" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J340" s="64" t="s">
+      <c r="J340" s="69" t="s">
         <v>343</v>
       </c>
       <c r="K340" s="15" t="s">
@@ -23089,7 +23115,7 @@
       <c r="I342" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J342" s="64"/>
+      <c r="J342" s="69"/>
       <c r="K342" s="15" t="s">
         <v>21</v>
       </c>
@@ -23143,7 +23169,7 @@
       <c r="I343" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J343" s="64"/>
+      <c r="J343" s="69"/>
       <c r="K343" s="15" t="s">
         <v>21</v>
       </c>
@@ -23197,7 +23223,7 @@
       <c r="I344" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J344" s="64" t="s">
+      <c r="J344" s="69" t="s">
         <v>343</v>
       </c>
       <c r="K344" s="15" t="s">
@@ -23253,7 +23279,7 @@
       <c r="I345" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J345" s="64" t="s">
+      <c r="J345" s="69" t="s">
         <v>630</v>
       </c>
       <c r="K345" s="15" t="s">
@@ -23309,7 +23335,7 @@
       <c r="I346" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J346" s="64" t="s">
+      <c r="J346" s="69" t="s">
         <v>343</v>
       </c>
       <c r="K346" s="15" t="s">
@@ -24226,7 +24252,7 @@
       <c r="I365" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J365" s="65" t="s">
+      <c r="J365" s="70" t="s">
         <v>327</v>
       </c>
       <c r="K365" s="15" t="s">
@@ -24910,7 +24936,7 @@
       <c r="I379" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J379" s="65" t="s">
+      <c r="J379" s="70" t="s">
         <v>327</v>
       </c>
       <c r="K379" s="15" t="s">
@@ -26207,7 +26233,7 @@
       <c r="I405" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J405" s="63" t="s">
+      <c r="J405" s="68" t="s">
         <v>327</v>
       </c>
       <c r="K405" s="15" t="s">
@@ -26712,7 +26738,7 @@
       <c r="I415" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J415" s="65" t="s">
+      <c r="J415" s="70" t="s">
         <v>327</v>
       </c>
       <c r="K415" s="15" t="s">
@@ -29521,7 +29547,7 @@
       <c r="I473" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J473" s="63" t="s">
+      <c r="J473" s="68" t="s">
         <v>327</v>
       </c>
       <c r="K473" s="15" t="s">
@@ -29662,36 +29688,36 @@
     </row>
     <row r="476" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A476" s="6"/>
-      <c r="B476" s="66"/>
-      <c r="C476" s="67"/>
-      <c r="D476" s="67"/>
+      <c r="B476" s="71"/>
+      <c r="C476" s="72"/>
+      <c r="D476" s="72"/>
       <c r="E476" s="6"/>
       <c r="F476" s="6"/>
       <c r="G476" s="6"/>
-      <c r="H476" s="68"/>
+      <c r="H476" s="73"/>
       <c r="I476" s="6"/>
-      <c r="J476" s="67"/>
-      <c r="K476" s="66"/>
-      <c r="L476" s="66"/>
-      <c r="M476" s="66"/>
-      <c r="N476" s="66"/>
-      <c r="O476" s="66"/>
-      <c r="P476" s="66"/>
-      <c r="Q476" s="66"/>
-      <c r="R476" s="66"/>
-      <c r="S476" s="66"/>
-      <c r="T476" s="66"/>
-      <c r="U476" s="66"/>
-      <c r="V476" s="66"/>
-      <c r="W476" s="66"/>
-      <c r="X476" s="66"/>
-      <c r="Y476" s="66"/>
-      <c r="Z476" s="66"/>
-      <c r="AA476" s="66"/>
-      <c r="AB476" s="66"/>
-      <c r="AC476" s="66"/>
-      <c r="AD476" s="66"/>
-      <c r="AE476" s="66"/>
+      <c r="J476" s="72"/>
+      <c r="K476" s="71"/>
+      <c r="L476" s="71"/>
+      <c r="M476" s="71"/>
+      <c r="N476" s="71"/>
+      <c r="O476" s="71"/>
+      <c r="P476" s="71"/>
+      <c r="Q476" s="71"/>
+      <c r="R476" s="71"/>
+      <c r="S476" s="71"/>
+      <c r="T476" s="71"/>
+      <c r="U476" s="71"/>
+      <c r="V476" s="71"/>
+      <c r="W476" s="71"/>
+      <c r="X476" s="71"/>
+      <c r="Y476" s="71"/>
+      <c r="Z476" s="71"/>
+      <c r="AA476" s="71"/>
+      <c r="AB476" s="71"/>
+      <c r="AC476" s="71"/>
+      <c r="AD476" s="71"/>
+      <c r="AE476" s="71"/>
     </row>
     <row r="477" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A477" s="9" t="s">
@@ -32989,7 +33015,7 @@
       <c r="I544" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J544" s="63" t="s">
+      <c r="J544" s="68" t="s">
         <v>327</v>
       </c>
       <c r="K544" s="15" t="s">
@@ -34897,7 +34923,7 @@
       <c r="I582" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J582" s="63" t="s">
+      <c r="J582" s="68" t="s">
         <v>327</v>
       </c>
       <c r="K582" s="15" t="s">
@@ -35903,7 +35929,7 @@
       <c r="I602" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J602" s="63" t="s">
+      <c r="J602" s="68" t="s">
         <v>327</v>
       </c>
       <c r="K602" s="15" t="s">
@@ -37768,7 +37794,7 @@
       <c r="I640" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J640" s="63" t="s">
+      <c r="J640" s="68" t="s">
         <v>327</v>
       </c>
       <c r="K640" s="15" t="s">
@@ -38571,7 +38597,7 @@
       <c r="I657" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J657" s="63" t="s">
+      <c r="J657" s="68" t="s">
         <v>327</v>
       </c>
       <c r="K657" s="15" t="s">
@@ -38799,39 +38825,39 @@
       <c r="AE661" s="4"/>
     </row>
     <row r="662" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A662" s="69" t="s">
+      <c r="A662" s="74" t="s">
         <v>1488</v>
       </c>
-      <c r="B662" s="69"/>
-      <c r="C662" s="69"/>
-      <c r="D662" s="69"/>
-      <c r="E662" s="69"/>
-      <c r="F662" s="69"/>
-      <c r="G662" s="69"/>
-      <c r="H662" s="69"/>
-      <c r="I662" s="69"/>
-      <c r="J662" s="69"/>
-      <c r="K662" s="69"/>
-      <c r="L662" s="66"/>
-      <c r="M662" s="66"/>
-      <c r="N662" s="66"/>
-      <c r="O662" s="66"/>
-      <c r="P662" s="66"/>
-      <c r="Q662" s="66"/>
-      <c r="R662" s="66"/>
-      <c r="S662" s="66"/>
-      <c r="T662" s="66"/>
-      <c r="U662" s="66"/>
-      <c r="V662" s="66"/>
-      <c r="W662" s="66"/>
-      <c r="X662" s="66"/>
-      <c r="Y662" s="66"/>
-      <c r="Z662" s="66"/>
-      <c r="AA662" s="66"/>
-      <c r="AB662" s="66"/>
-      <c r="AC662" s="66"/>
-      <c r="AD662" s="66"/>
-      <c r="AE662" s="66"/>
+      <c r="B662" s="74"/>
+      <c r="C662" s="74"/>
+      <c r="D662" s="74"/>
+      <c r="E662" s="74"/>
+      <c r="F662" s="74"/>
+      <c r="G662" s="74"/>
+      <c r="H662" s="74"/>
+      <c r="I662" s="74"/>
+      <c r="J662" s="74"/>
+      <c r="K662" s="74"/>
+      <c r="L662" s="71"/>
+      <c r="M662" s="71"/>
+      <c r="N662" s="71"/>
+      <c r="O662" s="71"/>
+      <c r="P662" s="71"/>
+      <c r="Q662" s="71"/>
+      <c r="R662" s="71"/>
+      <c r="S662" s="71"/>
+      <c r="T662" s="71"/>
+      <c r="U662" s="71"/>
+      <c r="V662" s="71"/>
+      <c r="W662" s="71"/>
+      <c r="X662" s="71"/>
+      <c r="Y662" s="71"/>
+      <c r="Z662" s="71"/>
+      <c r="AA662" s="71"/>
+      <c r="AB662" s="71"/>
+      <c r="AC662" s="71"/>
+      <c r="AD662" s="71"/>
+      <c r="AE662" s="71"/>
     </row>
     <row r="663" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A663" s="19" t="n">
@@ -38866,26 +38892,26 @@
       <c r="K663" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="L663" s="66"/>
-      <c r="M663" s="66"/>
-      <c r="N663" s="66"/>
-      <c r="O663" s="66"/>
-      <c r="P663" s="66"/>
-      <c r="Q663" s="66"/>
-      <c r="R663" s="66"/>
-      <c r="S663" s="66"/>
-      <c r="T663" s="66"/>
-      <c r="U663" s="66"/>
-      <c r="V663" s="66"/>
-      <c r="W663" s="66"/>
-      <c r="X663" s="66"/>
-      <c r="Y663" s="66"/>
-      <c r="Z663" s="66"/>
-      <c r="AA663" s="66"/>
-      <c r="AB663" s="66"/>
-      <c r="AC663" s="66"/>
-      <c r="AD663" s="66"/>
-      <c r="AE663" s="66"/>
+      <c r="L663" s="71"/>
+      <c r="M663" s="71"/>
+      <c r="N663" s="71"/>
+      <c r="O663" s="71"/>
+      <c r="P663" s="71"/>
+      <c r="Q663" s="71"/>
+      <c r="R663" s="71"/>
+      <c r="S663" s="71"/>
+      <c r="T663" s="71"/>
+      <c r="U663" s="71"/>
+      <c r="V663" s="71"/>
+      <c r="W663" s="71"/>
+      <c r="X663" s="71"/>
+      <c r="Y663" s="71"/>
+      <c r="Z663" s="71"/>
+      <c r="AA663" s="71"/>
+      <c r="AB663" s="71"/>
+      <c r="AC663" s="71"/>
+      <c r="AD663" s="71"/>
+      <c r="AE663" s="71"/>
     </row>
     <row r="664" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A664" s="19" t="n">
@@ -38922,26 +38948,26 @@
       <c r="K664" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="L664" s="66"/>
-      <c r="M664" s="66"/>
-      <c r="N664" s="66"/>
-      <c r="O664" s="66"/>
-      <c r="P664" s="66"/>
-      <c r="Q664" s="66"/>
-      <c r="R664" s="66"/>
-      <c r="S664" s="66"/>
-      <c r="T664" s="66"/>
-      <c r="U664" s="66"/>
-      <c r="V664" s="66"/>
-      <c r="W664" s="66"/>
-      <c r="X664" s="66"/>
-      <c r="Y664" s="66"/>
-      <c r="Z664" s="66"/>
-      <c r="AA664" s="66"/>
-      <c r="AB664" s="66"/>
-      <c r="AC664" s="66"/>
-      <c r="AD664" s="66"/>
-      <c r="AE664" s="66"/>
+      <c r="L664" s="71"/>
+      <c r="M664" s="71"/>
+      <c r="N664" s="71"/>
+      <c r="O664" s="71"/>
+      <c r="P664" s="71"/>
+      <c r="Q664" s="71"/>
+      <c r="R664" s="71"/>
+      <c r="S664" s="71"/>
+      <c r="T664" s="71"/>
+      <c r="U664" s="71"/>
+      <c r="V664" s="71"/>
+      <c r="W664" s="71"/>
+      <c r="X664" s="71"/>
+      <c r="Y664" s="71"/>
+      <c r="Z664" s="71"/>
+      <c r="AA664" s="71"/>
+      <c r="AB664" s="71"/>
+      <c r="AC664" s="71"/>
+      <c r="AD664" s="71"/>
+      <c r="AE664" s="71"/>
     </row>
     <row r="665" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A665" s="19" t="n">
@@ -38976,26 +39002,26 @@
       <c r="K665" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="L665" s="66"/>
-      <c r="M665" s="66"/>
-      <c r="N665" s="66"/>
-      <c r="O665" s="66"/>
-      <c r="P665" s="66"/>
-      <c r="Q665" s="66"/>
-      <c r="R665" s="66"/>
-      <c r="S665" s="66"/>
-      <c r="T665" s="66"/>
-      <c r="U665" s="66"/>
-      <c r="V665" s="66"/>
-      <c r="W665" s="66"/>
-      <c r="X665" s="66"/>
-      <c r="Y665" s="66"/>
-      <c r="Z665" s="66"/>
-      <c r="AA665" s="66"/>
-      <c r="AB665" s="66"/>
-      <c r="AC665" s="66"/>
-      <c r="AD665" s="66"/>
-      <c r="AE665" s="66"/>
+      <c r="L665" s="71"/>
+      <c r="M665" s="71"/>
+      <c r="N665" s="71"/>
+      <c r="O665" s="71"/>
+      <c r="P665" s="71"/>
+      <c r="Q665" s="71"/>
+      <c r="R665" s="71"/>
+      <c r="S665" s="71"/>
+      <c r="T665" s="71"/>
+      <c r="U665" s="71"/>
+      <c r="V665" s="71"/>
+      <c r="W665" s="71"/>
+      <c r="X665" s="71"/>
+      <c r="Y665" s="71"/>
+      <c r="Z665" s="71"/>
+      <c r="AA665" s="71"/>
+      <c r="AB665" s="71"/>
+      <c r="AC665" s="71"/>
+      <c r="AD665" s="71"/>
+      <c r="AE665" s="71"/>
     </row>
     <row r="666" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A666" s="19" t="n">
@@ -39030,26 +39056,26 @@
       <c r="K666" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="L666" s="66"/>
-      <c r="M666" s="66"/>
-      <c r="N666" s="66"/>
-      <c r="O666" s="66"/>
-      <c r="P666" s="66"/>
-      <c r="Q666" s="66"/>
-      <c r="R666" s="66"/>
-      <c r="S666" s="66"/>
-      <c r="T666" s="66"/>
-      <c r="U666" s="66"/>
-      <c r="V666" s="66"/>
-      <c r="W666" s="66"/>
-      <c r="X666" s="66"/>
-      <c r="Y666" s="66"/>
-      <c r="Z666" s="66"/>
-      <c r="AA666" s="66"/>
-      <c r="AB666" s="66"/>
-      <c r="AC666" s="66"/>
-      <c r="AD666" s="66"/>
-      <c r="AE666" s="66"/>
+      <c r="L666" s="71"/>
+      <c r="M666" s="71"/>
+      <c r="N666" s="71"/>
+      <c r="O666" s="71"/>
+      <c r="P666" s="71"/>
+      <c r="Q666" s="71"/>
+      <c r="R666" s="71"/>
+      <c r="S666" s="71"/>
+      <c r="T666" s="71"/>
+      <c r="U666" s="71"/>
+      <c r="V666" s="71"/>
+      <c r="W666" s="71"/>
+      <c r="X666" s="71"/>
+      <c r="Y666" s="71"/>
+      <c r="Z666" s="71"/>
+      <c r="AA666" s="71"/>
+      <c r="AB666" s="71"/>
+      <c r="AC666" s="71"/>
+      <c r="AD666" s="71"/>
+      <c r="AE666" s="71"/>
     </row>
     <row r="667" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A667" s="19" t="n">
@@ -39084,26 +39110,26 @@
       <c r="K667" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="L667" s="66"/>
-      <c r="M667" s="66"/>
-      <c r="N667" s="66"/>
-      <c r="O667" s="66"/>
-      <c r="P667" s="66"/>
-      <c r="Q667" s="66"/>
-      <c r="R667" s="66"/>
-      <c r="S667" s="66"/>
-      <c r="T667" s="66"/>
-      <c r="U667" s="66"/>
-      <c r="V667" s="66"/>
-      <c r="W667" s="66"/>
-      <c r="X667" s="66"/>
-      <c r="Y667" s="66"/>
-      <c r="Z667" s="66"/>
-      <c r="AA667" s="66"/>
-      <c r="AB667" s="66"/>
-      <c r="AC667" s="66"/>
-      <c r="AD667" s="66"/>
-      <c r="AE667" s="66"/>
+      <c r="L667" s="71"/>
+      <c r="M667" s="71"/>
+      <c r="N667" s="71"/>
+      <c r="O667" s="71"/>
+      <c r="P667" s="71"/>
+      <c r="Q667" s="71"/>
+      <c r="R667" s="71"/>
+      <c r="S667" s="71"/>
+      <c r="T667" s="71"/>
+      <c r="U667" s="71"/>
+      <c r="V667" s="71"/>
+      <c r="W667" s="71"/>
+      <c r="X667" s="71"/>
+      <c r="Y667" s="71"/>
+      <c r="Z667" s="71"/>
+      <c r="AA667" s="71"/>
+      <c r="AB667" s="71"/>
+      <c r="AC667" s="71"/>
+      <c r="AD667" s="71"/>
+      <c r="AE667" s="71"/>
     </row>
     <row r="668" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A668" s="19" t="n">
@@ -39138,26 +39164,26 @@
       <c r="K668" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="L668" s="66"/>
-      <c r="M668" s="66"/>
-      <c r="N668" s="66"/>
-      <c r="O668" s="66"/>
-      <c r="P668" s="66"/>
-      <c r="Q668" s="66"/>
-      <c r="R668" s="66"/>
-      <c r="S668" s="66"/>
-      <c r="T668" s="66"/>
-      <c r="U668" s="66"/>
-      <c r="V668" s="66"/>
-      <c r="W668" s="66"/>
-      <c r="X668" s="66"/>
-      <c r="Y668" s="66"/>
-      <c r="Z668" s="66"/>
-      <c r="AA668" s="66"/>
-      <c r="AB668" s="66"/>
-      <c r="AC668" s="66"/>
-      <c r="AD668" s="66"/>
-      <c r="AE668" s="66"/>
+      <c r="L668" s="71"/>
+      <c r="M668" s="71"/>
+      <c r="N668" s="71"/>
+      <c r="O668" s="71"/>
+      <c r="P668" s="71"/>
+      <c r="Q668" s="71"/>
+      <c r="R668" s="71"/>
+      <c r="S668" s="71"/>
+      <c r="T668" s="71"/>
+      <c r="U668" s="71"/>
+      <c r="V668" s="71"/>
+      <c r="W668" s="71"/>
+      <c r="X668" s="71"/>
+      <c r="Y668" s="71"/>
+      <c r="Z668" s="71"/>
+      <c r="AA668" s="71"/>
+      <c r="AB668" s="71"/>
+      <c r="AC668" s="71"/>
+      <c r="AD668" s="71"/>
+      <c r="AE668" s="71"/>
     </row>
     <row r="669" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A669" s="19" t="n">
@@ -39194,26 +39220,26 @@
       <c r="K669" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="L669" s="66"/>
-      <c r="M669" s="66"/>
-      <c r="N669" s="66"/>
-      <c r="O669" s="66"/>
-      <c r="P669" s="66"/>
-      <c r="Q669" s="66"/>
-      <c r="R669" s="66"/>
-      <c r="S669" s="66"/>
-      <c r="T669" s="66"/>
-      <c r="U669" s="66"/>
-      <c r="V669" s="66"/>
-      <c r="W669" s="66"/>
-      <c r="X669" s="66"/>
-      <c r="Y669" s="66"/>
-      <c r="Z669" s="66"/>
-      <c r="AA669" s="66"/>
-      <c r="AB669" s="66"/>
-      <c r="AC669" s="66"/>
-      <c r="AD669" s="66"/>
-      <c r="AE669" s="66"/>
+      <c r="L669" s="71"/>
+      <c r="M669" s="71"/>
+      <c r="N669" s="71"/>
+      <c r="O669" s="71"/>
+      <c r="P669" s="71"/>
+      <c r="Q669" s="71"/>
+      <c r="R669" s="71"/>
+      <c r="S669" s="71"/>
+      <c r="T669" s="71"/>
+      <c r="U669" s="71"/>
+      <c r="V669" s="71"/>
+      <c r="W669" s="71"/>
+      <c r="X669" s="71"/>
+      <c r="Y669" s="71"/>
+      <c r="Z669" s="71"/>
+      <c r="AA669" s="71"/>
+      <c r="AB669" s="71"/>
+      <c r="AC669" s="71"/>
+      <c r="AD669" s="71"/>
+      <c r="AE669" s="71"/>
     </row>
     <row r="670" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A670" s="29"/>
@@ -50372,28 +50398,28 @@
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
@@ -50431,19 +50457,19 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="76" t="s">
         <v>1516</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="n">
@@ -50488,7 +50514,7 @@
       <c r="B9" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="77" t="s">
         <v>1519</v>
       </c>
       <c r="D9" s="21" t="s">
@@ -50558,10 +50584,10 @@
       <c r="B11" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="78" t="s">
         <v>1523</v>
       </c>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="79" t="s">
         <v>1524</v>
       </c>
       <c r="E11" s="19" t="s">
@@ -50570,7 +50596,7 @@
       <c r="F11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="75" t="s">
+      <c r="G11" s="80" t="s">
         <v>1509</v>
       </c>
       <c r="H11" s="17" t="s">
@@ -50579,7 +50605,7 @@
       <c r="I11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="74"/>
+      <c r="J11" s="79"/>
       <c r="K11" s="15" t="s">
         <v>21</v>
       </c>
@@ -50592,10 +50618,10 @@
       <c r="B12" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="78" t="s">
         <v>1525</v>
       </c>
-      <c r="D12" s="74" t="s">
+      <c r="D12" s="79" t="s">
         <v>1526</v>
       </c>
       <c r="E12" s="19" t="s">
@@ -50604,7 +50630,7 @@
       <c r="F12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="75" t="s">
+      <c r="G12" s="80" t="s">
         <v>856</v>
       </c>
       <c r="H12" s="17" t="s">
@@ -50613,7 +50639,7 @@
       <c r="I12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="74"/>
+      <c r="J12" s="79"/>
       <c r="K12" s="15" t="s">
         <v>21</v>
       </c>
@@ -50626,10 +50652,10 @@
       <c r="B13" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="78" t="s">
         <v>1527</v>
       </c>
-      <c r="D13" s="74" t="s">
+      <c r="D13" s="79" t="s">
         <v>1528</v>
       </c>
       <c r="E13" s="19" t="s">
@@ -50638,7 +50664,7 @@
       <c r="F13" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="75" t="s">
+      <c r="G13" s="80" t="s">
         <v>748</v>
       </c>
       <c r="H13" s="17" t="s">
@@ -50647,7 +50673,7 @@
       <c r="I13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="74"/>
+      <c r="J13" s="79"/>
       <c r="K13" s="15" t="s">
         <v>21</v>
       </c>
@@ -50660,10 +50686,10 @@
       <c r="B14" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="73" t="s">
+      <c r="C14" s="78" t="s">
         <v>1529</v>
       </c>
-      <c r="D14" s="74" t="s">
+      <c r="D14" s="79" t="s">
         <v>1530</v>
       </c>
       <c r="E14" s="19" t="s">
@@ -50672,7 +50698,7 @@
       <c r="F14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="75" t="s">
+      <c r="G14" s="80" t="s">
         <v>66</v>
       </c>
       <c r="H14" s="17" t="s">
@@ -50681,7 +50707,7 @@
       <c r="I14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="74"/>
+      <c r="J14" s="79"/>
       <c r="K14" s="15" t="s">
         <v>21</v>
       </c>
@@ -50694,10 +50720,10 @@
       <c r="B15" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="78" t="s">
         <v>1531</v>
       </c>
-      <c r="D15" s="74" t="s">
+      <c r="D15" s="79" t="s">
         <v>1532</v>
       </c>
       <c r="E15" s="19" t="s">
@@ -50706,7 +50732,7 @@
       <c r="F15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="75" t="s">
+      <c r="G15" s="80" t="s">
         <v>1433</v>
       </c>
       <c r="H15" s="17" t="s">
@@ -50715,7 +50741,7 @@
       <c r="I15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="74"/>
+      <c r="J15" s="79"/>
       <c r="K15" s="15" t="s">
         <v>21</v>
       </c>
@@ -50728,10 +50754,10 @@
       <c r="B16" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="73" t="s">
+      <c r="C16" s="78" t="s">
         <v>1533</v>
       </c>
-      <c r="D16" s="74" t="s">
+      <c r="D16" s="79" t="s">
         <v>1534</v>
       </c>
       <c r="E16" s="19" t="s">
@@ -50740,7 +50766,7 @@
       <c r="F16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="75" t="s">
+      <c r="G16" s="80" t="s">
         <v>1535</v>
       </c>
       <c r="H16" s="17" t="s">
@@ -50749,7 +50775,7 @@
       <c r="I16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="74"/>
+      <c r="J16" s="79"/>
       <c r="K16" s="15" t="s">
         <v>21</v>
       </c>
@@ -50762,10 +50788,10 @@
       <c r="B17" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="73" t="s">
+      <c r="C17" s="78" t="s">
         <v>1536</v>
       </c>
-      <c r="D17" s="74" t="s">
+      <c r="D17" s="79" t="s">
         <v>1537</v>
       </c>
       <c r="E17" s="19" t="s">
@@ -50774,7 +50800,7 @@
       <c r="F17" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="75" t="s">
+      <c r="G17" s="80" t="s">
         <v>1538</v>
       </c>
       <c r="H17" s="17" t="s">
@@ -50783,7 +50809,7 @@
       <c r="I17" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="74" t="s">
+      <c r="J17" s="79" t="s">
         <v>1539</v>
       </c>
       <c r="K17" s="15" t="s">
@@ -50798,10 +50824,10 @@
       <c r="B18" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="73" t="s">
+      <c r="C18" s="78" t="s">
         <v>1540</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="79" t="s">
         <v>1541</v>
       </c>
       <c r="E18" s="19" t="s">
@@ -50810,7 +50836,7 @@
       <c r="F18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G18" s="75" t="s">
+      <c r="G18" s="80" t="s">
         <v>1542</v>
       </c>
       <c r="H18" s="17" t="s">
@@ -50819,7 +50845,7 @@
       <c r="I18" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="74"/>
+      <c r="J18" s="79"/>
       <c r="K18" s="15" t="s">
         <v>21</v>
       </c>
@@ -50832,10 +50858,10 @@
       <c r="B19" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="73" t="s">
+      <c r="C19" s="78" t="s">
         <v>1543</v>
       </c>
-      <c r="D19" s="74" t="s">
+      <c r="D19" s="79" t="s">
         <v>1544</v>
       </c>
       <c r="E19" s="19" t="s">
@@ -50844,7 +50870,7 @@
       <c r="F19" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G19" s="75" t="s">
+      <c r="G19" s="80" t="s">
         <v>1545</v>
       </c>
       <c r="H19" s="17" t="s">
@@ -50853,7 +50879,7 @@
       <c r="I19" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="74" t="s">
+      <c r="J19" s="79" t="s">
         <v>1546</v>
       </c>
       <c r="K19" s="15" t="s">
@@ -50868,10 +50894,10 @@
       <c r="B20" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="73" t="s">
+      <c r="C20" s="78" t="s">
         <v>1547</v>
       </c>
-      <c r="D20" s="74" t="s">
+      <c r="D20" s="79" t="s">
         <v>1548</v>
       </c>
       <c r="E20" s="19" t="s">
@@ -50880,7 +50906,7 @@
       <c r="F20" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G20" s="75" t="s">
+      <c r="G20" s="80" t="s">
         <v>1498</v>
       </c>
       <c r="H20" s="17" t="s">
@@ -50889,7 +50915,7 @@
       <c r="I20" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="74" t="s">
+      <c r="J20" s="79" t="s">
         <v>1549</v>
       </c>
       <c r="K20" s="15" t="s">
@@ -50904,10 +50930,10 @@
       <c r="B21" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="73" t="s">
+      <c r="C21" s="78" t="s">
         <v>1550</v>
       </c>
-      <c r="D21" s="74" t="s">
+      <c r="D21" s="79" t="s">
         <v>1551</v>
       </c>
       <c r="E21" s="19" t="s">
@@ -50916,7 +50942,7 @@
       <c r="F21" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="75" t="s">
+      <c r="G21" s="80" t="s">
         <v>1538</v>
       </c>
       <c r="H21" s="17" t="s">
@@ -50925,7 +50951,7 @@
       <c r="I21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="74" t="s">
+      <c r="J21" s="79" t="s">
         <v>1539</v>
       </c>
       <c r="K21" s="15" t="s">
@@ -50940,10 +50966,10 @@
       <c r="B22" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="73" t="s">
+      <c r="C22" s="78" t="s">
         <v>1552</v>
       </c>
-      <c r="D22" s="74" t="s">
+      <c r="D22" s="79" t="s">
         <v>1553</v>
       </c>
       <c r="E22" s="19" t="s">
@@ -50952,7 +50978,7 @@
       <c r="F22" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="75" t="s">
+      <c r="G22" s="80" t="s">
         <v>1542</v>
       </c>
       <c r="H22" s="17" t="s">
@@ -50961,7 +50987,7 @@
       <c r="I22" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J22" s="74"/>
+      <c r="J22" s="79"/>
       <c r="K22" s="15" t="s">
         <v>21</v>
       </c>
@@ -50974,10 +51000,10 @@
       <c r="B23" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="78" t="s">
         <v>1554</v>
       </c>
-      <c r="D23" s="74" t="s">
+      <c r="D23" s="79" t="s">
         <v>1555</v>
       </c>
       <c r="E23" s="19" t="s">
@@ -50986,7 +51012,7 @@
       <c r="F23" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G23" s="75" t="s">
+      <c r="G23" s="80" t="s">
         <v>1556</v>
       </c>
       <c r="H23" s="17" t="s">
@@ -50995,7 +51021,7 @@
       <c r="I23" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="74" t="s">
+      <c r="J23" s="79" t="s">
         <v>1557</v>
       </c>
       <c r="K23" s="15" t="s">
@@ -51007,13 +51033,13 @@
         <f aca="false">A23+1</f>
         <v>17</v>
       </c>
-      <c r="B24" s="76" t="s">
+      <c r="B24" s="81" t="s">
         <v>196</v>
       </c>
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="78" t="s">
         <v>1558</v>
       </c>
-      <c r="D24" s="74" t="s">
+      <c r="D24" s="79" t="s">
         <v>1559</v>
       </c>
       <c r="E24" s="14" t="s">
@@ -51022,7 +51048,7 @@
       <c r="F24" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G24" s="75" t="s">
+      <c r="G24" s="80" t="s">
         <v>18</v>
       </c>
       <c r="H24" s="17" t="s">
@@ -51031,7 +51057,7 @@
       <c r="I24" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="74"/>
+      <c r="J24" s="79"/>
       <c r="K24" s="15" t="s">
         <v>21</v>
       </c>
@@ -51041,22 +51067,22 @@
         <f aca="false">A24+1</f>
         <v>18</v>
       </c>
-      <c r="B25" s="76" t="s">
+      <c r="B25" s="81" t="s">
         <v>1560</v>
       </c>
-      <c r="C25" s="73" t="s">
+      <c r="C25" s="78" t="s">
         <v>1561</v>
       </c>
-      <c r="D25" s="74" t="s">
+      <c r="D25" s="79" t="s">
         <v>1562</v>
       </c>
       <c r="E25" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="75" t="s">
+      <c r="F25" s="80" t="s">
         <v>196</v>
       </c>
-      <c r="G25" s="75" t="s">
+      <c r="G25" s="80" t="s">
         <v>1563</v>
       </c>
       <c r="H25" s="17" t="s">
@@ -51065,7 +51091,7 @@
       <c r="I25" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="74"/>
+      <c r="J25" s="79"/>
       <c r="K25" s="15" t="s">
         <v>21</v>
       </c>
@@ -51075,22 +51101,22 @@
         <f aca="false">A25+1</f>
         <v>19</v>
       </c>
-      <c r="B26" s="76" t="s">
+      <c r="B26" s="81" t="s">
         <v>1564</v>
       </c>
-      <c r="C26" s="73" t="s">
+      <c r="C26" s="78" t="s">
         <v>1565</v>
       </c>
-      <c r="D26" s="74" t="s">
+      <c r="D26" s="79" t="s">
         <v>1566</v>
       </c>
       <c r="E26" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="75" t="s">
+      <c r="F26" s="80" t="s">
         <v>196</v>
       </c>
-      <c r="G26" s="75" t="s">
+      <c r="G26" s="80" t="s">
         <v>1542</v>
       </c>
       <c r="H26" s="17" t="s">
@@ -51099,7 +51125,7 @@
       <c r="I26" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J26" s="74"/>
+      <c r="J26" s="79"/>
       <c r="K26" s="15" t="s">
         <v>21</v>
       </c>
@@ -51109,13 +51135,13 @@
         <f aca="false">A26+1</f>
         <v>20</v>
       </c>
-      <c r="B27" s="77" t="s">
+      <c r="B27" s="82" t="s">
         <v>234</v>
       </c>
-      <c r="C27" s="78" t="s">
+      <c r="C27" s="83" t="s">
         <v>1567</v>
       </c>
-      <c r="D27" s="79" t="s">
+      <c r="D27" s="84" t="s">
         <v>1568</v>
       </c>
       <c r="E27" s="24" t="s">
@@ -51124,7 +51150,7 @@
       <c r="F27" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G27" s="80" t="s">
+      <c r="G27" s="85" t="s">
         <v>18</v>
       </c>
       <c r="H27" s="27" t="s">
@@ -51133,7 +51159,7 @@
       <c r="I27" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="J27" s="79" t="s">
+      <c r="J27" s="84" t="s">
         <v>1568</v>
       </c>
       <c r="K27" s="25" t="s">
@@ -51145,34 +51171,34 @@
         <f aca="false">A27+1</f>
         <v>21</v>
       </c>
-      <c r="B28" s="77" t="s">
+      <c r="B28" s="82" t="s">
         <v>1569</v>
       </c>
-      <c r="C28" s="78" t="s">
+      <c r="C28" s="83" t="s">
         <v>1570</v>
       </c>
-      <c r="D28" s="79" t="s">
+      <c r="D28" s="84" t="s">
         <v>1571</v>
       </c>
       <c r="E28" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F28" s="80" t="s">
+      <c r="F28" s="85" t="s">
         <v>234</v>
       </c>
-      <c r="G28" s="80" t="s">
+      <c r="G28" s="85" t="s">
         <v>1572</v>
       </c>
-      <c r="H28" s="80" t="s">
+      <c r="H28" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="I28" s="80" t="s">
+      <c r="I28" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="J28" s="79" t="s">
+      <c r="J28" s="84" t="s">
         <v>1573</v>
       </c>
-      <c r="K28" s="77" t="s">
+      <c r="K28" s="82" t="s">
         <v>21</v>
       </c>
     </row>
@@ -51181,34 +51207,34 @@
         <f aca="false">A28+1</f>
         <v>22</v>
       </c>
-      <c r="B29" s="77" t="s">
+      <c r="B29" s="82" t="s">
         <v>1574</v>
       </c>
-      <c r="C29" s="78" t="s">
+      <c r="C29" s="83" t="s">
         <v>1575</v>
       </c>
-      <c r="D29" s="79" t="s">
+      <c r="D29" s="84" t="s">
         <v>1576</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="80" t="s">
+      <c r="F29" s="85" t="s">
         <v>234</v>
       </c>
-      <c r="G29" s="80" t="s">
+      <c r="G29" s="85" t="s">
         <v>1572</v>
       </c>
-      <c r="H29" s="80" t="s">
+      <c r="H29" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="80" t="s">
+      <c r="I29" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="J29" s="79" t="s">
+      <c r="J29" s="84" t="s">
         <v>1577</v>
       </c>
-      <c r="K29" s="77" t="s">
+      <c r="K29" s="82" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>